<commit_message>
squashed some bugs. updated the formulas. updates the calculate not to produce an excel, but instead display everything in the webpage.
</commit_message>
<xml_diff>
--- a/static/excel/manuel.xlsx
+++ b/static/excel/manuel.xlsx
@@ -124,7 +124,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>789</v>
+        <v>482</v>
       </c>
     </row>
     <row r="10" spans="2:3">
@@ -132,7 +132,7 @@
         <v>4</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>631.2</v>
+        <v>385.6</v>
       </c>
     </row>
     <row r="11" spans="2:3">
@@ -140,7 +140,7 @@
         <v>5</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>725.88</v>
+        <v>443.44</v>
       </c>
     </row>
     <row r="12" spans="2:3">
@@ -148,7 +148,7 @@
         <v>6</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:3">
@@ -156,7 +156,7 @@
         <v>7</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>650.88</v>
+        <v>443.44</v>
       </c>
     </row>
     <row r="14" spans="2:3">
@@ -164,7 +164,7 @@
         <v>8</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>72.32</v>
+        <v>443.44</v>
       </c>
     </row>
     <row r="15" spans="2:3">

</xml_diff>